<commit_message>
feat(visualisasi_cluster): add annual tren graphics
</commit_message>
<xml_diff>
--- a/assets/files/Dataset_Clustering_Wilayah.xlsx
+++ b/assets/files/Dataset_Clustering_Wilayah.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansC\Documents\Coding\Skripsi\Experiment\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD50FE7-0C13-4255-97FE-B5BF09E3AA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A581EC2-44CB-450F-9589-EC08A52BA997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1935,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1543"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A978" workbookViewId="0">
+      <selection activeCell="N999" sqref="N999"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>